<commit_message>
Update base model version to match final EPS 2.1.1-us-v2
</commit_message>
<xml_diff>
--- a/InputData/cpi.xlsx
+++ b/InputData/cpi.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robbie\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-1.4.2-us - AEO Update\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74B894A-F356-4233-B257-22D3D9ACBC5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="135" windowWidth="20100" windowHeight="7410" activeTab="1"/>
+    <workbookView xWindow="5310" yWindow="1590" windowWidth="21660" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
   <si>
     <t>CPI Consumer Price Index</t>
   </si>
@@ -238,13 +249,16 @@
     <t>2018.............................................................................     .</t>
   </si>
   <si>
-    <t>https://www.bls.gov/cpi/tables/supplemental-files/historical-cpi-u-201812.pdf</t>
+    <t>2019.............................................................................     .</t>
+  </si>
+  <si>
+    <t>https://www.bls.gov/cpi/tables/supplemental-files/historical-cpi-u-201912.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -403,6 +417,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -438,6 +469,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -613,12 +661,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -637,7 +683,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -647,7 +693,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -677,7 +723,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -685,12 +731,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1228,7 +1272,7 @@
         <v>4.2</v>
       </c>
       <c r="G29" s="6">
-        <f t="shared" ref="G29:G56" si="0">$D$50/D29</f>
+        <f t="shared" ref="G29:G57" si="0">$D$50/D29</f>
         <v>1.6857121879588841</v>
       </c>
       <c r="M29" s="1"/>
@@ -1963,6 +2007,30 @@
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" s="4"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57">
+        <v>254.41200000000001</v>
+      </c>
+      <c r="C57">
+        <v>256.90300000000002</v>
+      </c>
+      <c r="D57">
+        <v>255.65700000000001</v>
+      </c>
+      <c r="E57">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F57">
+        <v>1.8</v>
+      </c>
+      <c r="G57" s="6">
+        <f t="shared" si="0"/>
+        <v>0.89805481563188172</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Returning BAU subsidies to zero
</commit_message>
<xml_diff>
--- a/InputData/cpi.xlsx
+++ b/InputData/cpi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\US_EPS\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire Trevisan\Dropbox (Energy Innovation)\Documents\GitHub\eps-eu\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59485A2-ADF5-4469-ABB4-3A063C7F174B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BBEE27-531B-4D8E-B966-2CBF55DA3417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="1620" windowWidth="12720" windowHeight="14955" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
   <si>
     <t>CPI Consumer Price Index</t>
   </si>
@@ -256,6 +256,12 @@
   </si>
   <si>
     <t>2020............................................................................. .</t>
+  </si>
+  <si>
+    <t>2021............................................................................. .</t>
+  </si>
+  <si>
+    <t>2022............................................................................. .</t>
   </si>
 </sst>
 </file>
@@ -671,14 +677,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -686,42 +692,42 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -737,34 +743,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
-    <col min="15" max="15" width="28.140625" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" customWidth="1"/>
+    <col min="15" max="15" width="28.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -781,7 +787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -795,7 +801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -815,7 +821,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -835,7 +841,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -855,7 +861,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -875,7 +881,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -895,7 +901,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -915,7 +921,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -935,7 +941,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -955,7 +961,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -975,7 +981,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -995,7 +1001,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1015,7 +1021,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1035,7 +1041,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1055,7 +1061,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1075,7 +1081,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1095,7 +1101,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -1115,7 +1121,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1135,7 +1141,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1155,7 +1161,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -1175,7 +1181,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -1195,7 +1201,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -1215,7 +1221,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -1235,7 +1241,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>1.7566488140780414</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -1279,14 +1285,14 @@
         <v>4.2</v>
       </c>
       <c r="G29" s="6">
-        <f t="shared" ref="G29:G57" si="0">$D$50/D29</f>
+        <f t="shared" ref="G29:G56" si="0">$D$50/D29</f>
         <v>1.6857121879588841</v>
       </c>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1313,7 +1319,7 @@
       <c r="N30" s="2"/>
       <c r="O30" s="4"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -1340,7 +1346,7 @@
       <c r="N31" s="2"/>
       <c r="O31" s="4"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1367,7 +1373,7 @@
       <c r="N32" s="2"/>
       <c r="O32" s="4"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -1394,7 +1400,7 @@
       <c r="N33" s="2"/>
       <c r="O33" s="4"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -1421,7 +1427,7 @@
       <c r="N34" s="2"/>
       <c r="O34" s="4"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -1448,7 +1454,7 @@
       <c r="N35" s="2"/>
       <c r="O35" s="4"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -1475,7 +1481,7 @@
       <c r="N36" s="2"/>
       <c r="O36" s="4"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -1502,7 +1508,7 @@
       <c r="N37" s="2"/>
       <c r="O37" s="4"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -1529,7 +1535,7 @@
       <c r="N38" s="5"/>
       <c r="O38" s="4"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -1556,7 +1562,7 @@
       <c r="N39" s="2"/>
       <c r="O39" s="4"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -1583,7 +1589,7 @@
       <c r="N40" s="2"/>
       <c r="O40" s="4"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>57</v>
       </c>
@@ -1610,7 +1616,7 @@
       <c r="N41" s="2"/>
       <c r="O41" s="4"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -1637,7 +1643,7 @@
       <c r="N42" s="2"/>
       <c r="O42" s="4"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>59</v>
       </c>
@@ -1664,7 +1670,7 @@
       <c r="N43" s="5"/>
       <c r="O43" s="4"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>60</v>
       </c>
@@ -1691,7 +1697,7 @@
       <c r="N44" s="2"/>
       <c r="O44" s="4"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>61</v>
       </c>
@@ -1718,7 +1724,7 @@
       <c r="N45" s="2"/>
       <c r="O45" s="4"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>62</v>
       </c>
@@ -1745,7 +1751,7 @@
       <c r="N46" s="2"/>
       <c r="O46" s="4"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>63</v>
       </c>
@@ -1772,7 +1778,7 @@
       <c r="N47" s="2"/>
       <c r="O47" s="4"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>64</v>
       </c>
@@ -1799,7 +1805,7 @@
       <c r="N48" s="2"/>
       <c r="O48" s="4"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>65</v>
       </c>
@@ -1826,7 +1832,7 @@
       <c r="N49" s="2"/>
       <c r="O49" s="4"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>66</v>
       </c>
@@ -1853,7 +1859,7 @@
       <c r="N50" s="2"/>
       <c r="O50" s="4"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>67</v>
       </c>
@@ -1880,7 +1886,7 @@
       <c r="N51" s="2"/>
       <c r="O51" s="4"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>68</v>
       </c>
@@ -1907,7 +1913,7 @@
       <c r="N52" s="2"/>
       <c r="O52" s="4"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>69</v>
       </c>
@@ -1934,7 +1940,7 @@
       <c r="N53" s="2"/>
       <c r="O53" s="4"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>70</v>
       </c>
@@ -1961,7 +1967,7 @@
       <c r="N54" s="2"/>
       <c r="O54" s="4"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>71</v>
       </c>
@@ -1988,7 +1994,7 @@
       <c r="N55" s="2"/>
       <c r="O55" s="4"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>72</v>
       </c>
@@ -2008,14 +2014,14 @@
         <v>2.4</v>
       </c>
       <c r="G56" s="6">
-        <f t="shared" si="0"/>
+        <f>$D$50/D56</f>
         <v>0.9143273584567535</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" s="4"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>73</v>
       </c>
@@ -2039,7 +2045,7 @@
         <v>0.89805481563188172</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>74</v>
       </c>
@@ -2061,6 +2067,30 @@
       <c r="G58" s="6">
         <f>$D$50/D58</f>
         <v>0.88711067149387013</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>75</v>
+      </c>
+      <c r="D59">
+        <v>270.96975000000003</v>
+      </c>
+      <c r="G59" s="6">
+        <f t="shared" ref="G59:G60" si="1">$D$50/D59</f>
+        <v>0.84730491134157948</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>76</v>
+      </c>
+      <c r="D60">
+        <v>292.27836363636362</v>
+      </c>
+      <c r="G60" s="6">
+        <f>$D$50/D60</f>
+        <v>0.78553197418898923</v>
       </c>
     </row>
   </sheetData>

</xml_diff>